<commit_message>
Clash Identification and Resolving- PREUPDATING
</commit_message>
<xml_diff>
--- a/database/schoolInfo.xlsx
+++ b/database/schoolInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\Iron_\PycharmProjects\NEA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\Iron_\NEA Project 1.2\NEA_Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC9F6CC-2E29-4D34-A1EB-1499125F455F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3FFE5C-EFCB-4E4E-8EF5-3A4DE7AB54F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3086A932-FA98-4602-9749-498EA20A41DC}"/>
+    <workbookView xWindow="135" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{3086A932-FA98-4602-9749-498EA20A41DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="61">
   <si>
     <t>Pupil ID</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Obama</t>
-  </si>
-  <si>
-    <t>Alternative Site</t>
   </si>
   <si>
     <t>MY005</t>
@@ -705,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225CECA0-6E50-48E0-95CD-6DA68B4975DD}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>29</v>
       </c>
@@ -1053,10 +1050,10 @@
         <v>38046</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>29</v>
       </c>
@@ -1073,10 +1070,10 @@
         <v>38046</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>29</v>
       </c>
@@ -1093,10 +1090,10 @@
         <v>38046</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -1113,10 +1110,10 @@
         <v>38046</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -1133,18 +1130,18 @@
         <v>38046</v>
       </c>
       <c r="F21" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>9</v>
@@ -1158,13 +1155,13 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>12</v>
@@ -1176,18 +1173,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="E24" s="6">
         <v>37506</v>
@@ -1196,15 +1193,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>27</v>
@@ -1216,15 +1213,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>28</v>
@@ -1238,13 +1235,13 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
@@ -1258,13 +1255,13 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>11</v>
@@ -1278,16 +1275,16 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="D29" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="12">
         <v>37637</v>
@@ -1298,13 +1295,13 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>28</v>
@@ -1318,13 +1315,13 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>14</v>
@@ -1338,13 +1335,13 @@
     </row>
     <row r="32" spans="1:6" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>18</v>
@@ -1358,13 +1355,13 @@
     </row>
     <row r="33" spans="1:6" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>12</v>
@@ -1378,13 +1375,13 @@
     </row>
     <row r="34" spans="1:6" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>20</v>
@@ -1398,13 +1395,13 @@
     </row>
     <row r="35" spans="1:6" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>21</v>
@@ -1418,13 +1415,13 @@
     </row>
     <row r="36" spans="1:6" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>14</v>
@@ -1438,13 +1435,13 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C37" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>9</v>
@@ -1458,16 +1455,16 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C38" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="E38" s="12">
         <v>37274</v>
@@ -1478,13 +1475,13 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C39" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>13</v>
@@ -1498,13 +1495,13 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C40" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>28</v>
@@ -1518,13 +1515,13 @@
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C41" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>14</v>
@@ -1536,15 +1533,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>9</v>
@@ -1556,15 +1553,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>26</v>
@@ -1578,13 +1575,13 @@
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>13</v>
@@ -1596,15 +1593,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>20</v>
@@ -1616,15 +1613,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
@@ -1638,13 +1635,13 @@
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>9</v>
@@ -1658,13 +1655,13 @@
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>12</v>
@@ -1678,16 +1675,16 @@
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="C49" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="D49" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E49" s="12">
         <v>37642</v>
@@ -1698,13 +1695,13 @@
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>21</v>
@@ -1718,13 +1715,13 @@
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>14</v>
@@ -1736,15 +1733,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>9</v>
@@ -1758,13 +1755,13 @@
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>12</v>
@@ -1776,15 +1773,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>21</v>
@@ -1796,15 +1793,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>28</v>
@@ -1816,15 +1813,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>14</v>
@@ -1858,18 +1855,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8">
         <v>2</v>
@@ -1880,7 +1877,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="8">
         <v>3</v>
@@ -1891,7 +1888,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="8">
         <v>5</v>
@@ -1902,7 +1899,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="8">
         <v>2</v>
@@ -1913,7 +1910,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="8">
         <v>10</v>

</xml_diff>